<commit_message>
Proveravamo da li nesto ostalo za komitovanje
</commit_message>
<xml_diff>
--- a/racun.xlsx
+++ b/racun.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>datum</t>
   </si>
@@ -55,12 +55,36 @@
   </si>
   <si>
     <t>60 min</t>
+  </si>
+  <si>
+    <t>245 min</t>
+  </si>
+  <si>
+    <t>230 min</t>
+  </si>
+  <si>
+    <t>280 min</t>
+  </si>
+  <si>
+    <t>305 min</t>
+  </si>
+  <si>
+    <t>345 min</t>
+  </si>
+  <si>
+    <t>450 min</t>
+  </si>
+  <si>
+    <t>45 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -115,20 +139,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,252 +460,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:G30"/>
+  <dimension ref="B3:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>11.06</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>1800</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>14.06</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>1800</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>17.059999999999999</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>1800</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>24.06</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>2800</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>30.06</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="5">
         <v>2400</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>1.07</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <v>2200</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>14.07</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="5">
         <v>3000</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>15.07</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="5">
         <v>500</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <v>16.07</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>2200</v>
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>17.07</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <v>2200</v>
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>18.07</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>1000</v>
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <v>19.07</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <v>1200</v>
       </c>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>20.07</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="6">
         <v>2400</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1">
-        <f>SUM(D4:D16)</f>
-        <v>25300</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="1">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:7">
+    <row r="17" spans="2:4">
+      <c r="B17" s="3">
+        <v>21.07</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="3">
+        <v>29.07</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="7">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="3">
+        <v>30.07</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="3">
+        <v>2.08</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="7">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="3">
+        <v>3.08</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="7">
+        <v>6010</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="3">
+        <v>4.08</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="3">
+        <v>6.08</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="7">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="3">
+        <v>9.08</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="7">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="3">
+        <v>10.08</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="8">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:7">
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="2:4">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:7">
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="2:4">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:7">
+      <c r="C28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="11">
+        <f>SUM(D4:D25)</f>
+        <v>67210</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:7">
+      <c r="C29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="11">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>